<commit_message>
add graphics and table
</commit_message>
<xml_diff>
--- a/matmul/MatMul.xlsx
+++ b/matmul/MatMul.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\79372\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lyaki\OneDrive\Рабочий стол\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C6091A-53D2-4BB1-B761-662FB9E6A630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06B1C8D-5DBA-4142-973B-DE77FD8681D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -27,16 +27,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Размер матриц</t>
+    <t>Acceleration</t>
   </si>
   <si>
-    <t>CPU, с</t>
+    <t>Dimension</t>
   </si>
   <si>
-    <t>GPU, с</t>
+    <t>GPU Time,c</t>
   </si>
   <si>
-    <t>Ускорение</t>
+    <t>CPU Time,c</t>
   </si>
 </sst>
 </file>
@@ -72,8 +72,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -126,11 +129,23 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="ru-RU"/>
-              <a:t>Умножение</a:t>
+              <a:t>Время</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="ru-RU" baseline="0"/>
-              <a:t> матриц</a:t>
+              <a:t> работы на </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>GPU </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t>и на </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>CPU</a:t>
             </a:r>
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
@@ -172,12 +187,23 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GPU Time,c</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -188,10 +214,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$21</c:f>
+              <c:f>Лист1!$A$2:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -199,127 +225,37 @@
                   <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>1600</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$D$2:$D$21</c:f>
+              <c:f>Лист1!$B$2:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>15.09433962264151</c:v>
+                  <c:v>6.2299999999999996E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.045454545454543</c:v>
+                  <c:v>7.8200000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.154471544715449</c:v>
+                  <c:v>2.2460000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.728813559322038</c:v>
+                  <c:v>1.7448000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.333333333333329</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32.24431818181818</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>38.511796733212336</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>31.086691086691083</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>37.466777408637874</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>38.961038961038959</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>53.80952380952381</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>39.187739463601531</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>59.43962848297214</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>59.634969325153371</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>74.854166666666671</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>76.870689655172413</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>88.809187279151942</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>80.96546310832025</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>97.237908496732018</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>84.177438307873103</c:v>
+                  <c:v>0.101769</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -327,7 +263,88 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D34E-4E0A-8D26-81AE06D8A3EA}"/>
+              <c16:uniqueId val="{00000001-1863-462F-A1CB-B50E6F917B8F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPU Time,c</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.6979999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.628E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33167099999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7089639999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.214314999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1863-462F-A1CB-B50E6F917B8F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -340,16 +357,44 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1410829615"/>
-        <c:axId val="1538799967"/>
+        <c:axId val="326171088"/>
+        <c:axId val="326164968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1410829615"/>
+        <c:axId val="326171088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -371,7 +416,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="ru-RU"/>
-                  <a:t>Размер матриц</a:t>
+                  <a:t>Размерность</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -442,15 +487,520 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1538799967"/>
+        <c:crossAx val="326164968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1538799967"/>
+        <c:axId val="326164968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Время,</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> с</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="326171088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Ускорение</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Acceleration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$D$2:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.5409309791332264</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.393861892583118</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>147.67186108637577</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>155.25928473177439</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>454.10994507168192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B3C4-4E64-AEAF-5330DCD12187}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="494968456"/>
+        <c:axId val="494972416"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="494968456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Размерность</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="494972416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="494972416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,7 +1106,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1410829615"/>
+        <c:crossAx val="494968456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -568,6 +1118,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -652,6 +1233,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1168,27 +1789,543 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Диаграмма 1">
+        <xdr:cNvPr id="5" name="Диаграмма 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75856A31-2EE5-293F-EA83-4CC6E836CA7D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD1DEB7F-D2F7-4A1E-35F2-371FF46063CB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1206,21 +2343,43 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Диаграмма 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A038ABB9-0699-7BFD-8578-AE00C9FB59C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9CD38A7-B33C-42C2-A9C6-E1E5CE9EE01C}" name="Таблица1" displayName="Таблица1" ref="A1:D21" totalsRowShown="0">
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D2E20B12-3CDC-4011-B15B-5ACB8720A039}" name="Размер матриц"/>
-    <tableColumn id="2" xr3:uid="{D94E0C8B-0F18-4351-8D44-91D03A780509}" name="CPU, с"/>
-    <tableColumn id="3" xr3:uid="{7DFAFE64-366E-4806-8F79-215C0B1F5545}" name="GPU, с"/>
-    <tableColumn id="4" xr3:uid="{955548E7-EF47-45BA-867C-BA8588C2C3C5}" name="Ускорение">
-      <calculatedColumnFormula>B2/C2</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1486,337 +2645,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>100</v>
       </c>
-      <c r="B2">
-        <v>4.0000000000000001E-3</v>
+      <c r="B2" s="1">
+        <v>6.2299999999999996E-4</v>
       </c>
-      <c r="C2">
-        <v>2.6499999999999999E-4</v>
+      <c r="C2" s="1">
+        <v>4.6979999999999999E-3</v>
       </c>
-      <c r="D2">
-        <f>B2/C2</f>
-        <v>15.09433962264151</v>
+      <c r="D2" s="1">
+        <f>$C2/$B2</f>
+        <v>7.5409309791332264</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>200</v>
       </c>
-      <c r="B3">
-        <v>0.03</v>
+      <c r="B3" s="1">
+        <v>7.8200000000000003E-4</v>
       </c>
-      <c r="C3">
-        <v>1.7600000000000001E-3</v>
+      <c r="C3" s="1">
+        <v>3.628E-2</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D21" si="0">B3/C3</f>
-        <v>17.045454545454543</v>
+      <c r="D3" s="1">
+        <f>$C3/$B3</f>
+        <v>46.393861892583118</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>300</v>
+      <c r="A4" s="1">
+        <v>400</v>
       </c>
-      <c r="B4">
-        <v>0.109</v>
+      <c r="B4" s="1">
+        <v>2.2460000000000002E-3</v>
       </c>
-      <c r="C4">
-        <v>4.9199999999999999E-3</v>
+      <c r="C4" s="1">
+        <v>0.33167099999999999</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>22.154471544715449</v>
+      <c r="D4" s="1">
+        <f>$C4/$B4</f>
+        <v>147.67186108637577</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>400</v>
+      <c r="A5" s="1">
+        <v>800</v>
       </c>
-      <c r="B5">
-        <v>0.28000000000000003</v>
+      <c r="B5" s="1">
+        <v>1.7448000000000002E-2</v>
       </c>
-      <c r="C5">
-        <v>1.18E-2</v>
+      <c r="C5" s="1">
+        <v>2.7089639999999999</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>23.728813559322038</v>
+      <c r="D5" s="1">
+        <f>$C5/$B5</f>
+        <v>155.25928473177439</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>500</v>
-      </c>
-      <c r="B6">
-        <v>0.57799999999999996</v>
-      </c>
-      <c r="C6">
-        <v>2.0400000000000001E-2</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>28.333333333333329</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>600</v>
-      </c>
-      <c r="B7">
-        <v>1.135</v>
-      </c>
-      <c r="C7">
-        <v>3.5200000000000002E-2</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>32.24431818181818</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>700</v>
-      </c>
-      <c r="B8">
-        <v>2.1219999999999999</v>
-      </c>
-      <c r="C8">
-        <v>5.5100000000000003E-2</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>38.511796733212336</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>800</v>
-      </c>
-      <c r="B9">
-        <v>2.5459999999999998</v>
-      </c>
-      <c r="C9">
-        <v>8.1900000000000001E-2</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>31.086691086691083</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>900</v>
-      </c>
-      <c r="B10">
-        <v>4.5110000000000001</v>
-      </c>
-      <c r="C10">
-        <v>0.12039999999999999</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>37.466777408637874</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>1000</v>
-      </c>
-      <c r="B11">
-        <v>6.3</v>
-      </c>
-      <c r="C11">
-        <v>0.16170000000000001</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>38.961038961038959</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>1100</v>
-      </c>
-      <c r="B12">
-        <v>10.17</v>
-      </c>
-      <c r="C12">
-        <v>0.189</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>53.80952380952381</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>1200</v>
-      </c>
-      <c r="B13">
-        <v>10.228</v>
-      </c>
-      <c r="C13">
-        <v>0.26100000000000001</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>39.187739463601531</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>1300</v>
-      </c>
-      <c r="B14">
-        <v>19.199000000000002</v>
-      </c>
-      <c r="C14">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>59.43962848297214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>1400</v>
-      </c>
-      <c r="B15">
-        <v>19.440999999999999</v>
-      </c>
-      <c r="C15">
-        <v>0.32600000000000001</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>59.634969325153371</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>1500</v>
-      </c>
-      <c r="B16">
-        <v>32.337000000000003</v>
-      </c>
-      <c r="C16">
-        <v>0.432</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>74.854166666666671</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A6" s="1">
         <v>1600</v>
       </c>
-      <c r="B17">
-        <v>35.667999999999999</v>
+      <c r="B6" s="1">
+        <v>0.101769</v>
       </c>
-      <c r="C17">
-        <v>0.46400000000000002</v>
+      <c r="C6" s="1">
+        <v>46.214314999999999</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>76.870689655172413</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>1700</v>
-      </c>
-      <c r="B18">
-        <v>50.265999999999998</v>
-      </c>
-      <c r="C18">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>88.809187279151942</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>1800</v>
-      </c>
-      <c r="B19">
-        <v>51.575000000000003</v>
-      </c>
-      <c r="C19">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>80.96546310832025</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>1900</v>
-      </c>
-      <c r="B20">
-        <v>74.387</v>
-      </c>
-      <c r="C20">
-        <v>0.76500000000000001</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>97.237908496732018</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>2000</v>
-      </c>
-      <c r="B21">
-        <v>71.635000000000005</v>
-      </c>
-      <c r="C21">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>84.177438307873103</v>
+      <c r="D6" s="1">
+        <f>$C6/$B6</f>
+        <v>454.10994507168192</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>